<commit_message>
Lecture de fichier csv pour récupérer les emails
</commit_message>
<xml_diff>
--- a/src/Web/wwwroot/fichiers/Templates_Formation_Invitation.xlsx
+++ b/src/Web/wwwroot/fichiers/Templates_Formation_Invitation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1939379\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\session6\ProjetIntegrateur\projetBlog\gwenael\src\Web\wwwroot\fichiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72527BBB-BEA7-4355-B1D4-83BBAADE6394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810CDA7C-61BC-44C0-9DB2-400F262C6057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,7 +90,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -99,7 +99,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -132,22 +138,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,7 +437,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B3:B4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,22 +448,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="3"/>
@@ -466,10 +472,10 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>

</xml_diff>